<commit_message>
add visualisation for text analyssi & conditions
</commit_message>
<xml_diff>
--- a/interviews_corrected/structured_data_manual.xlsx
+++ b/interviews_corrected/structured_data_manual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Meditation-Interviews\src\audio_and_experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Meditation-Interviews\interviews_corrected\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C321F772-DA90-4940-92D8-9FFEE1D714D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C961FA45-714F-4662-872D-ADA65F53C8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D7D4240-F1F1-462A-A574-7C1F6EBCACE7}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{3D7D4240-F1F1-462A-A574-7C1F6EBCACE7}"/>
   </bookViews>
   <sheets>
     <sheet name="structured_data_manual" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="99">
   <si>
     <t>Experiment</t>
   </si>
   <si>
-    <t>File_name</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>Order_Condition</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -311,6 +302,21 @@
   </si>
   <si>
     <t>Moslty empty</t>
+  </si>
+  <si>
+    <t>S301final</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Order Condition</t>
   </si>
 </sst>
 </file>
@@ -1201,40 +1207,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC2A6DB-C6FD-412D-9D85-CA9107A99F38}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1242,16 +1252,19 @@
       <c r="D2" s="1">
         <v>7.1180555555555554E-3</v>
       </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -1259,13 +1272,19 @@
       <c r="D3" s="1">
         <v>6.6898148148148151E-3</v>
       </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -1273,13 +1292,19 @@
       <c r="D4" s="1">
         <v>2.7893518518518519E-3</v>
       </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -1287,16 +1312,19 @@
       <c r="D5" s="1">
         <v>3.1712962962962962E-3</v>
       </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
       <c r="F5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>13</v>
@@ -1304,13 +1332,19 @@
       <c r="D6" s="1">
         <v>5.0810185185185186E-3</v>
       </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>13</v>
@@ -1318,13 +1352,19 @@
       <c r="D7" s="1">
         <v>2.3263888888888887E-3</v>
       </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -1332,16 +1372,19 @@
       <c r="D8" s="1">
         <v>1.9907407407407408E-3</v>
       </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>15</v>
@@ -1349,16 +1392,19 @@
       <c r="D9" s="1">
         <v>1.2152777777777778E-3</v>
       </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
       <c r="F9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1366,16 +1412,19 @@
       <c r="D10" s="1">
         <v>1.8171296296296297E-3</v>
       </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
       <c r="F10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>17</v>
@@ -1383,16 +1432,19 @@
       <c r="D11" s="1">
         <v>2.0601851851851853E-3</v>
       </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
       <c r="F11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>18</v>
@@ -1400,16 +1452,19 @@
       <c r="D12" s="1">
         <v>2.1643518518518518E-3</v>
       </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
       <c r="F12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>19</v>
@@ -1417,13 +1472,19 @@
       <c r="D13" s="1">
         <v>4.1550925925925922E-3</v>
       </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>19</v>
@@ -1431,13 +1492,19 @@
       <c r="D14" s="1">
         <v>2.7893518518518519E-3</v>
       </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -1445,16 +1512,19 @@
       <c r="D15" s="1">
         <v>2.1064814814814813E-3</v>
       </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
       <c r="F15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>22</v>
@@ -1462,16 +1532,19 @@
       <c r="D16" s="1">
         <v>3.3796296296296296E-3</v>
       </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
       <c r="F16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>23</v>
@@ -1479,16 +1552,19 @@
       <c r="D17" s="1">
         <v>4.0625000000000001E-3</v>
       </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
       <c r="F17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>24</v>
@@ -1496,13 +1572,19 @@
       <c r="D18" s="1">
         <v>1.3888888888888889E-3</v>
       </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>24</v>
@@ -1510,13 +1592,19 @@
       <c r="D19" s="1">
         <v>3.1828703703703702E-3</v>
       </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>201</v>
@@ -1525,18 +1613,18 @@
         <v>3.2986111111111111E-3</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>201</v>
@@ -1545,18 +1633,18 @@
         <v>8.9583333333333338E-3</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>201</v>
@@ -1565,18 +1653,18 @@
         <v>1.5509259259259259E-3</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>202</v>
@@ -1585,7 +1673,7 @@
         <v>6.6435185185185182E-3</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1593,10 +1681,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>203</v>
@@ -1605,7 +1693,7 @@
         <v>4.2824074074074075E-3</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1613,10 +1701,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>204</v>
@@ -1625,18 +1713,18 @@
         <v>5.4398148148148144E-4</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>204</v>
@@ -1645,18 +1733,18 @@
         <v>3.5185185185185185E-3</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>205</v>
@@ -1665,18 +1753,18 @@
         <v>3.5879629629629629E-4</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>205</v>
@@ -1685,18 +1773,18 @@
         <v>4.4675925925925924E-3</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>206</v>
@@ -1705,18 +1793,18 @@
         <v>7.8703703703703705E-4</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C30">
         <v>206</v>
@@ -1725,18 +1813,18 @@
         <v>2.2106481481481482E-3</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>207</v>
@@ -1745,18 +1833,18 @@
         <v>1.2152777777777778E-3</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C32">
         <v>207</v>
@@ -1765,18 +1853,18 @@
         <v>4.3981481481481481E-4</v>
       </c>
       <c r="E32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C33">
         <v>208</v>
@@ -1785,18 +1873,18 @@
         <v>1.0717592592592593E-2</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>208</v>
@@ -1805,18 +1893,18 @@
         <v>4.5138888888888885E-3</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C35">
         <v>209</v>
@@ -1825,18 +1913,18 @@
         <v>5.7291666666666663E-3</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>209</v>
@@ -1845,7 +1933,7 @@
         <v>4.2013888888888891E-3</v>
       </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1853,10 +1941,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C37">
         <v>209</v>
@@ -1865,7 +1953,7 @@
         <v>4.0509259259259257E-3</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1873,10 +1961,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>209</v>
@@ -1885,18 +1973,18 @@
         <v>9.5949074074074079E-3</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>210</v>
@@ -1905,18 +1993,18 @@
         <v>1.9791666666666668E-3</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C40">
         <v>210</v>
@@ -1925,7 +2013,7 @@
         <v>6.1921296296296299E-3</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1933,10 +2021,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C41">
         <v>210</v>
@@ -1945,18 +2033,18 @@
         <v>9.1435185185185178E-3</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F41" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>211</v>
@@ -1965,18 +2053,18 @@
         <v>4.5254629629629629E-3</v>
       </c>
       <c r="E42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F42" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>211</v>
@@ -1985,7 +2073,7 @@
         <v>3.0092592592592593E-3</v>
       </c>
       <c r="E43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1993,10 +2081,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>211</v>
@@ -2005,18 +2093,18 @@
         <v>5.185185185185185E-3</v>
       </c>
       <c r="E44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C45">
         <v>212</v>
@@ -2025,18 +2113,18 @@
         <v>2.488425925925926E-3</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F45" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C46">
         <v>212</v>
@@ -2045,18 +2133,18 @@
         <v>5.4861111111111109E-3</v>
       </c>
       <c r="E46" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F46" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C47">
         <v>213</v>
@@ -2065,21 +2153,21 @@
         <v>1.5277777777777779E-3</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>213</v>
@@ -2088,18 +2176,18 @@
         <v>3.0671296296296297E-3</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C49">
         <v>214</v>
@@ -2108,18 +2196,18 @@
         <v>1.3657407407407407E-3</v>
       </c>
       <c r="E49" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C50">
         <v>214</v>
@@ -2128,18 +2216,18 @@
         <v>7.407407407407407E-4</v>
       </c>
       <c r="E50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C51">
         <v>217</v>
@@ -2148,7 +2236,7 @@
         <v>7.7777777777777776E-3</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2156,10 +2244,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C52">
         <v>218</v>
@@ -2168,18 +2256,18 @@
         <v>2.5925925925925925E-3</v>
       </c>
       <c r="E52" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F52" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C53">
         <v>218</v>
@@ -2188,18 +2276,18 @@
         <v>2.8124999999999999E-3</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F53" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C54">
         <v>219</v>
@@ -2208,21 +2296,21 @@
         <v>1.1226851851851851E-3</v>
       </c>
       <c r="E54" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F54" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C55">
         <v>219</v>
@@ -2231,18 +2319,18 @@
         <v>2.7662037037037039E-3</v>
       </c>
       <c r="E55" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F55" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C56">
         <v>220</v>
@@ -2251,18 +2339,18 @@
         <v>2.0138888888888888E-3</v>
       </c>
       <c r="E56" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C57">
         <v>220</v>
@@ -2271,18 +2359,18 @@
         <v>2.476851851851852E-3</v>
       </c>
       <c r="E57" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C58">
         <v>222</v>
@@ -2291,18 +2379,18 @@
         <v>4.8726851851851848E-3</v>
       </c>
       <c r="E58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C59">
         <v>222</v>
@@ -2311,18 +2399,18 @@
         <v>5.5787037037037038E-3</v>
       </c>
       <c r="E59" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C60">
         <v>223</v>
@@ -2331,7 +2419,7 @@
         <v>2.7546296296296294E-3</v>
       </c>
       <c r="E60" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2339,10 +2427,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C61">
         <v>225</v>
@@ -2351,21 +2439,21 @@
         <v>1.273148148148148E-4</v>
       </c>
       <c r="E61" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>225</v>
@@ -2374,18 +2462,18 @@
         <v>1.2141203703703704E-2</v>
       </c>
       <c r="E62" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C63">
         <v>226</v>
@@ -2394,21 +2482,21 @@
         <v>5.0925925925925921E-4</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C64">
         <v>226</v>
@@ -2417,7 +2505,7 @@
         <v>2.8935185185185184E-4</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2425,10 +2513,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C65">
         <v>226</v>
@@ -2437,7 +2525,7 @@
         <v>2.638888888888889E-3</v>
       </c>
       <c r="E65" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2445,10 +2533,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C66">
         <v>227</v>
@@ -2457,18 +2545,18 @@
         <v>1.6435185185185185E-3</v>
       </c>
       <c r="E66" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F66" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C67">
         <v>227</v>
@@ -2477,18 +2565,18 @@
         <v>4.0740740740740737E-3</v>
       </c>
       <c r="E67" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F67" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C68">
         <v>228</v>
@@ -2497,18 +2585,18 @@
         <v>3.3912037037037036E-3</v>
       </c>
       <c r="E68" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F68" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C69">
         <v>228</v>
@@ -2517,18 +2605,18 @@
         <v>5.8564814814814816E-3</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F69" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C70">
         <v>229</v>
@@ -2537,18 +2625,18 @@
         <v>3.5995370370370369E-3</v>
       </c>
       <c r="E70" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F70" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C71">
         <v>229</v>
@@ -2557,18 +2645,18 @@
         <v>7.3842592592592597E-3</v>
       </c>
       <c r="E71" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F71" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C72">
         <v>230</v>
@@ -2577,18 +2665,18 @@
         <v>1.9791666666666668E-3</v>
       </c>
       <c r="E72" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F72" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C73">
         <v>230</v>
@@ -2597,47 +2685,47 @@
         <v>4.9884259259259257E-3</v>
       </c>
       <c r="E73" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F73" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C74">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D74" s="1">
-        <v>2.9166666666666668E-3</v>
+        <v>4.3518518518518515E-3</v>
       </c>
       <c r="E74" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" t="s">
-        <v>31</v>
+        <v>95</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C75">
         <v>302</v>
       </c>
       <c r="D75" s="1">
-        <v>2.6967592592592594E-3</v>
+        <v>2.9166666666666668E-3</v>
       </c>
       <c r="E75" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F75" t="s">
         <v>28</v>
@@ -2645,39 +2733,39 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C76">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D76" s="1">
-        <v>5.8564814814814816E-3</v>
+        <v>2.6967592592592594E-3</v>
       </c>
       <c r="E76" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F76" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" t="s">
         <v>86</v>
-      </c>
-      <c r="B77" t="s">
-        <v>90</v>
       </c>
       <c r="C77">
         <v>303</v>
       </c>
       <c r="D77" s="1">
-        <v>3.1712962962962962E-3</v>
+        <v>5.8564814814814816E-3</v>
       </c>
       <c r="E77" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F77" t="s">
         <v>28</v>
@@ -2685,79 +2773,79 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C78">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D78" s="1">
-        <v>4.9189814814814816E-3</v>
+        <v>3.1712962962962962E-3</v>
       </c>
       <c r="E78" t="s">
-        <v>33</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="F78" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C79">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D79" s="1">
-        <v>1.1689814814814816E-3</v>
+        <v>4.9189814814814816E-3</v>
       </c>
       <c r="E79" t="s">
-        <v>33</v>
-      </c>
-      <c r="F79" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C80">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D80" s="1">
-        <v>6.1342592592592594E-3</v>
+        <v>1.1689814814814816E-3</v>
       </c>
       <c r="E80" t="s">
-        <v>27</v>
-      </c>
-      <c r="F80">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="F80" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C81">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D81" s="1">
-        <v>4.340277777777778E-3</v>
+        <v>6.1342592592592594E-3</v>
       </c>
       <c r="E81" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -2765,29 +2853,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C82">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D82" s="1">
-        <v>6.6666666666666671E-3</v>
+        <v>4.340277777777778E-3</v>
       </c>
       <c r="E82" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
     </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83">
+        <v>313</v>
+      </c>
+      <c r="D83" s="1">
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="E83" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F82 G44 G47 G54">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="F1:F2 F5 F8:F12 F15:F17 F20:F83 G47 G54">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2800,5 +2905,25 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{793A369C-F563-4F72-826D-BF7D3E8BE128}">
+            <xm:f>NOT(ISERROR(SEARCH(0,F1)))</xm:f>
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F1:F2 F5 F8:F12 F15:F17 F20:F83 G47 G54</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add condtions for OBE1 & stripplot align by ID
</commit_message>
<xml_diff>
--- a/interviews_corrected/structured_data_manual.xlsx
+++ b/interviews_corrected/structured_data_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Meditation-Interviews\interviews_corrected\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C961FA45-714F-4662-872D-ADA65F53C8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629698F-B171-442A-9A5A-F006FCF74033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{3D7D4240-F1F1-462A-A574-7C1F6EBCACE7}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{3D7D4240-F1F1-462A-A574-7C1F6EBCACE7}"/>
   </bookViews>
   <sheets>
     <sheet name="structured_data_manual" sheetId="1" r:id="rId1"/>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1253,7 @@
         <v>7.1180555555555554E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1273,10 +1273,10 @@
         <v>6.6898148148148151E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,10 +1293,10 @@
         <v>2.7893518518518519E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1313,7 +1313,7 @@
         <v>3.1712962962962962E-3</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1333,10 +1333,10 @@
         <v>5.0810185185185186E-3</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1353,10 +1353,10 @@
         <v>2.3263888888888887E-3</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1373,7 +1373,7 @@
         <v>1.9907407407407408E-3</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1393,7 +1393,7 @@
         <v>1.2152777777777778E-3</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1413,7 +1413,7 @@
         <v>1.8171296296296297E-3</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1433,7 +1433,7 @@
         <v>2.0601851851851853E-3</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1453,7 +1453,7 @@
         <v>2.1643518518518518E-3</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1473,10 +1473,10 @@
         <v>4.1550925925925922E-3</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1493,10 +1493,10 @@
         <v>2.7893518518518519E-3</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,7 +1513,7 @@
         <v>2.1064814814814813E-3</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1533,7 +1533,7 @@
         <v>3.3796296296296296E-3</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1573,10 +1573,10 @@
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1593,10 +1593,10 @@
         <v>3.1828703703703702E-3</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>